<commit_message>
log updates: chlorosis, burns, and dark adapted fluorescence
</commit_message>
<xml_diff>
--- a/logs/general_schedule.xlsx
+++ b/logs/general_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monik\Documents\git\2025_TT_psf\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01C7360-20BE-44CD-B8D8-62EDB433D44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853338B4-6A82-4ABD-A09A-873C1C21124E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{0E8C84BF-39F7-498C-9A68-8E5CF28203AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E8C84BF-39F7-498C-9A68-8E5CF28203AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>date</t>
   </si>
@@ -87,6 +87,30 @@
   </si>
   <si>
     <t>large number of trillium individuals have emerged</t>
+  </si>
+  <si>
+    <t>Watering schedule every Monday &amp; Thursday, unless stated. 100mL each time</t>
+  </si>
+  <si>
+    <t>Isotope every Wednesday, unless stated. 20mL each time</t>
+  </si>
+  <si>
+    <t>did not water</t>
+  </si>
+  <si>
+    <t>worried about overwatering potentially, skipped day</t>
+  </si>
+  <si>
+    <t>some trillium are starting to yellow at tips</t>
+  </si>
+  <si>
+    <t>some trillium showing burn marks</t>
+  </si>
+  <si>
+    <t>trillium yellowing</t>
+  </si>
+  <si>
+    <t>trillium burning</t>
   </si>
 </sst>
 </file>
@@ -459,20 +483,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0DE265-7766-4628-AAFB-F23C0C3E3508}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45946</v>
       </c>
@@ -499,8 +523,11 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45951</v>
       </c>
@@ -513,8 +540,11 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45964</v>
       </c>
@@ -528,7 +558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45964</v>
       </c>
@@ -542,7 +572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45973</v>
       </c>
@@ -554,6 +584,42 @@
       </c>
       <c r="D6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45992</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45989</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>